<commit_message>
acg project 108 part 1
</commit_message>
<xml_diff>
--- a/Developer/developer_log.xlsx
+++ b/Developer/developer_log.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3BE5BA-E887-4A5A-A5D0-9E0E29297DDF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B41F143-5431-4D5F-B053-1B6441477CA4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="810" windowWidth="14610" windowHeight="13665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="570" windowWidth="22290" windowHeight="13665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -249,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -332,6 +332,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -341,7 +344,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -627,35 +630,36 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8:Q9"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="G1" s="31" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="1" t="s">
@@ -681,19 +685,19 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
+      <c r="A2" s="32">
         <v>43755</v>
       </c>
-      <c r="B2" s="35">
+      <c r="B2" s="32">
         <v>43756</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="36">
         <v>43757</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="36">
         <v>43758</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="36">
         <v>43759</v>
       </c>
       <c r="F2" s="4">
@@ -801,11 +805,21 @@
         <v>17</v>
       </c>
       <c r="K4" s="22"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="20"/>
+      <c r="L4" s="10">
+        <v>43758</v>
+      </c>
+      <c r="M4" s="14">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="N4" s="14">
+        <v>0.9375</v>
+      </c>
+      <c r="O4" s="18">
+        <v>3</v>
+      </c>
+      <c r="P4" s="20">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -944,15 +958,15 @@
       <c r="P8" s="20"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="35"/>
       <c r="I9" s="5">
         <v>8</v>
       </c>

</xml_diff>